<commit_message>
Kinder Morning Walkthrough (Spoilers)
</commit_message>
<xml_diff>
--- a/quicktype/Text Adventures/WorkInProgress/Kinder/Locations.xlsx
+++ b/quicktype/Text Adventures/WorkInProgress/Kinder/Locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cool_\Documents\trs80mc10\quicktype\Text Adventures\WorkInProgress\Kinder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FC75E359-D996-4D88-BBDA-F56F9DCA7302}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6A01A26F-DF5A-49DB-9953-8095DD75BC83}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7350" xr2:uid="{0D7CC9F5-48AA-4D50-90AC-57B063EE6F5B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="21">
   <si>
     <t>FOREST</t>
   </si>
@@ -69,13 +69,25 @@
     <t>FRONT</t>
   </si>
   <si>
-    <t>TUNNEL</t>
-  </si>
-  <si>
     <t>LAKESIDE</t>
   </si>
   <si>
     <t>GULLY</t>
+  </si>
+  <si>
+    <t>W TUNNEL</t>
+  </si>
+  <si>
+    <t>E TUNNEL</t>
+  </si>
+  <si>
+    <t>CLEARING</t>
+  </si>
+  <si>
+    <t>CAMPSITE</t>
+  </si>
+  <si>
+    <t>PIPLINEE</t>
   </si>
 </sst>
 </file>
@@ -128,6 +140,151 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F3B6549-1248-4C4E-B7B4-955F7160652D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1200150" y="2286000"/>
+          <a:ext cx="3876675" cy="5505450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>Walkthrough:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>E,GET BAG</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>W,W,W,GET PAPER,READ PAPER</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>N,W,W,W,S,W,W,N</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>(GO</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t> NORTH and GO SOUTH until  chipmunk comes)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>GIVE BAG (or THROW PEANUTS)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>S (BACK ONTO TRAIL. If bear shows up, GO UP. If moose, WAIT. These tactics work for any forest location)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>E,E,E,S,S,E,E,E,E,GET FLASHLIGHT,W,W,W,W,W,N,N,N</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>UNLOCK DOOR,N</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>EXAMINE LEVER,READ PAPER (Notice that the paper is the reverse of what you see when you EXAMINE LEVER), TURN PAPER (Note the direction, left or right, indicated after turning the paper--that's the real solution)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>PUSH LEVEL (WHICH DIRECTION?),the direction indicated after issuing the command TURN PAPER</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -429,11 +586,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AAE8F2F-2B80-4762-BABA-0826C7EE9C57}">
   <dimension ref="A2:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2">
@@ -472,7 +635,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -490,7 +653,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J3" t="s">
         <v>1</v>
@@ -522,7 +685,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J4" t="s">
         <v>1</v>
@@ -554,7 +717,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J5" t="s">
         <v>1</v>
@@ -586,7 +749,7 @@
         <v>3</v>
       </c>
       <c r="I6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J6" t="s">
         <v>1</v>
@@ -600,10 +763,10 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
         <v>3</v>
@@ -632,7 +795,7 @@
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -650,7 +813,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J8" t="s">
         <v>1</v>
@@ -664,25 +827,25 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G9" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="I9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J9" t="s">
         <v>1</v>
@@ -696,7 +859,7 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -714,7 +877,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J10" t="s">
         <v>1</v>
@@ -722,5 +885,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>